<commit_message>
prototype for NiCd allocated process
</commit_message>
<xml_diff>
--- a/data/lci_data/lci-batt_lci.xlsx
+++ b/data/lci_data/lci-batt_lci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="32">
   <si>
     <t>Database</t>
   </si>
@@ -31,7 +31,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>f3e14ff1-4e03-4f47-8ed3-ca7fe48f05a7</t>
+    <t>70ee3a39-0833-4d35-b404-a39e9bff7b97</t>
   </si>
   <si>
     <t>location</t>
@@ -70,13 +70,28 @@
     <t>nickel-metal hybride battery recovery slag 2</t>
   </si>
   <si>
-    <t>076c9af2-f2b6-47b1-ba90-87c9e40e3113</t>
+    <t>098fcc52-e3ec-490a-beb3-c05c7d07f218</t>
   </si>
   <si>
     <t>nickel-metal hybride battery waste</t>
   </si>
   <si>
-    <t>369c0dd3-5bd8-43dc-8ab2-ac3200f366f7</t>
+    <t>4953ef88-d5d5-4523-9b2e-b7e66cc3ae2e</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>market for copper smelting facility</t>
+  </si>
+  <si>
+    <t>GLO</t>
+  </si>
+  <si>
+    <t>technosphere</t>
+  </si>
+  <si>
+    <t>ecoinvent treatment of Ni-metal hybride battery</t>
   </si>
   <si>
     <t>market group for electricity, medium voltage</t>
@@ -85,19 +100,16 @@
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>technosphere</t>
-  </si>
-  <si>
     <t>recovered ferrous scrap</t>
   </si>
   <si>
     <t>recovered nickel</t>
   </si>
   <si>
-    <t>5299f521-3b05-4ebd-ae02-3fd54e23d994</t>
-  </si>
-  <si>
-    <t>5e404637-d154-4b40-b482-42030e3f2bdd</t>
+    <t>6ab66874-3b7f-4c77-8601-719cb6ea6438</t>
+  </si>
+  <si>
+    <t>053574a8-569f-4fdd-b61a-4053f9a313f5</t>
   </si>
 </sst>
 </file>
@@ -438,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -571,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -579,7 +591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -587,12 +599,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -609,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -626,7 +638,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -634,7 +646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -642,7 +654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -650,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -658,7 +670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -666,7 +678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -674,12 +686,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -695,8 +707,11 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -713,262 +728,285 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B32">
-        <v>0.066</v>
+        <v>5E-10</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>0.31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>-0</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>-0.1091723014830094</v>
       </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
         <v>24</v>
       </c>
-      <c r="B35">
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36">
         <v>-0.5083601468312615</v>
       </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36">
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
         <v>-0.2535257812778481</v>
       </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
+      <c r="B39" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>8</v>
       </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
         <v>9</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>11</v>
       </c>
-      <c r="B43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>15</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>6</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>11</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46">
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47">
         <v>1</v>
       </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" t="s">
-        <v>27</v>
+      <c r="B49" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="s">
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57">
         <v>1</v>
       </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>